<commit_message>
fix the sheet to show the trendline
</commit_message>
<xml_diff>
--- a/bootstrap_method.xlsx
+++ b/bootstrap_method.xlsx
@@ -270,18 +270,26 @@
             </spPr>
           </marker>
           <trendline>
+            <spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:srgbClr val="FF0000"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
             <trendlineType val="linear"/>
             <dispRSqr val="1"/>
             <dispEq val="1"/>
           </trendline>
           <xVal>
             <numRef>
-              <f>'Flight Tests → CD0, e'!$J$31:$J$43</f>
+              <f>'Flight Tests → CD0, e'!$J$32:$J$43</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'Flight Tests → CD0, e'!$I$31:$I$43</f>
+              <f>'Flight Tests → CD0, e'!$I$32:$I$43</f>
             </numRef>
           </yVal>
         </ser>
@@ -391,12 +399,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>'Flight Tests → CD0, e'!$E$31:$E$43</f>
+              <f>'Flight Tests → CD0, e'!$E$32:$E$43</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'Flight Tests → CD0, e'!$H$31:$H$43</f>
+              <f>'Flight Tests → CD0, e'!$H$32:$H$43</f>
             </numRef>
           </yVal>
         </ser>
@@ -506,12 +514,12 @@
           </marker>
           <xVal>
             <numRef>
-              <f>'Flight Tests → CD0, e'!$E$63:$E$75</f>
+              <f>'Flight Tests → CD0, e'!$E$64:$E$75</f>
             </numRef>
           </xVal>
           <yVal>
             <numRef>
-              <f>'Flight Tests → CD0, e'!$G$63:$G$75</f>
+              <f>'Flight Tests → CD0, e'!$G$64:$G$75</f>
             </numRef>
           </yVal>
         </ser>

</xml_diff>

<commit_message>
remove the fit line that doesnt show
</commit_message>
<xml_diff>
--- a/bootstrap_method.xlsx
+++ b/bootstrap_method.xlsx
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -142,7 +142,6 @@
     <xf numFmtId="167" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="166" fontId="0" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="170" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -278,36 +277,6 @@
           <yVal>
             <numRef>
               <f>'Flight Tests → CD0, e'!$I$32:$I$43</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Linear fit (R² in B56)</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Flight Tests → CD0, e'!$J$59:$J$60</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Flight Tests → CD0, e'!$I$59:$I$60</f>
             </numRef>
           </yVal>
         </ser>
@@ -2940,31 +2909,6 @@
         </is>
       </c>
     </row>
-    <row r="59">
-      <c r="H59" s="25" t="inlineStr">
-        <is>
-          <t>Fit line:</t>
-        </is>
-      </c>
-      <c r="I59" s="18">
-        <f>IF(COUNT(I32:I43)&gt;1,B47*MIN(J32:J43)+B48,"")</f>
-        <v/>
-      </c>
-      <c r="J59" s="19">
-        <f>IF(COUNT(J32:J43)&gt;1,MIN(J32:J43),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="60">
-      <c r="I60" s="18">
-        <f>IF(COUNT(I32:I43)&gt;1,B47*MAX(J32:J43)+B48,"")</f>
-        <v/>
-      </c>
-      <c r="J60" s="19">
-        <f>IF(COUNT(J32:J43)&gt;1,MAX(J32:J43),"")</f>
-        <v/>
-      </c>
-    </row>
     <row r="62">
       <c r="A62" s="2" t="inlineStr">
         <is>
@@ -3506,7 +3450,7 @@
           <t>S (wing area)</t>
         </is>
       </c>
-      <c r="B5" s="26" t="n">
+      <c r="B5" s="25" t="n">
         <v>174</v>
       </c>
       <c r="C5" s="14" t="inlineStr">
@@ -3526,7 +3470,7 @@
           <t>B (wing span)</t>
         </is>
       </c>
-      <c r="B6" s="26" t="n">
+      <c r="B6" s="25" t="n">
         <v>36</v>
       </c>
       <c r="C6" s="14" t="inlineStr">
@@ -3546,7 +3490,7 @@
           <t>P0 (rated power)</t>
         </is>
       </c>
-      <c r="B7" s="26" t="n">
+      <c r="B7" s="25" t="n">
         <v>235</v>
       </c>
       <c r="C7" s="14" t="inlineStr">
@@ -3566,7 +3510,7 @@
           <t>N0 (rated RPM)</t>
         </is>
       </c>
-      <c r="B8" s="26" t="n">
+      <c r="B8" s="25" t="n">
         <v>2400</v>
       </c>
       <c r="C8" s="14" t="inlineStr">
@@ -3586,7 +3530,7 @@
           <t>d (prop diameter)</t>
         </is>
       </c>
-      <c r="B9" s="26" t="n">
+      <c r="B9" s="25" t="n">
         <v>6.83</v>
       </c>
       <c r="C9" s="14" t="inlineStr">
@@ -3657,7 +3601,7 @@
           <t>Z (fuselage dia / prop dia)</t>
         </is>
       </c>
-      <c r="B13" s="26" t="n">
+      <c r="B13" s="25" t="n">
         <v>0.6879999999999999</v>
       </c>
       <c r="C13" s="14" t="inlineStr"/>
@@ -3673,7 +3617,7 @@
           <t>Tractor? (1=yes, 0=no)</t>
         </is>
       </c>
-      <c r="B14" s="26" t="n">
+      <c r="B14" s="25" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="14" t="inlineStr"/>
@@ -3689,7 +3633,7 @@
           <t>BB (num blades)</t>
         </is>
       </c>
-      <c r="B15" s="26" t="n">
+      <c r="B15" s="25" t="n">
         <v>2</v>
       </c>
       <c r="C15" s="14" t="inlineStr"/>
@@ -3705,7 +3649,7 @@
           <t>C (power dropoff)</t>
         </is>
       </c>
-      <c r="B16" s="26" t="n">
+      <c r="B16" s="25" t="n">
         <v>0.12</v>
       </c>
       <c r="C16" s="14" t="inlineStr"/>
@@ -3757,188 +3701,188 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="27" t="inlineStr">
+      <c r="A21" s="26" t="inlineStr">
         <is>
           <t>{:S</t>
         </is>
       </c>
-      <c r="B21" s="27">
+      <c r="B21" s="26">
         <f>TEXT(B5,"0.0")</f>
         <v/>
       </c>
-      <c r="C21" s="27" t="inlineStr">
+      <c r="C21" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; wing area, ft²</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="27" t="inlineStr">
+      <c r="A22" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :B</t>
         </is>
       </c>
-      <c r="B22" s="27">
+      <c r="B22" s="26">
         <f>TEXT(B6,"0.0")</f>
         <v/>
       </c>
-      <c r="C22" s="27" t="inlineStr">
+      <c r="C22" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; wing span, ft</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="27" t="inlineStr">
+      <c r="A23" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :P0</t>
         </is>
       </c>
-      <c r="B23" s="27">
+      <c r="B23" s="26">
         <f>TEXT(B7,"0.0")</f>
         <v/>
       </c>
-      <c r="C23" s="27" t="inlineStr">
+      <c r="C23" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; rated MSL power, hp</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="27" t="inlineStr">
+      <c r="A24" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :N0</t>
         </is>
       </c>
-      <c r="B24" s="27">
+      <c r="B24" s="26">
         <f>TEXT(B8,"0")</f>
         <v/>
       </c>
-      <c r="C24" s="27" t="inlineStr">
+      <c r="C24" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; rated RPM</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="27" t="inlineStr">
+      <c r="A25" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :d</t>
         </is>
       </c>
-      <c r="B25" s="27">
+      <c r="B25" s="26">
         <f>TEXT(B9,"0.000")</f>
         <v/>
       </c>
-      <c r="C25" s="27" t="inlineStr">
+      <c r="C25" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; prop diameter, ft</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="27" t="inlineStr">
+      <c r="A26" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :CD0</t>
         </is>
       </c>
-      <c r="B26" s="27">
+      <c r="B26" s="26">
         <f>TEXT(B10,"0.00000")</f>
         <v/>
       </c>
-      <c r="C26" s="27" t="inlineStr">
+      <c r="C26" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; parasite drag coefficient</t>
         </is>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="27" t="inlineStr">
+      <c r="A27" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :e</t>
         </is>
       </c>
-      <c r="B27" s="27">
+      <c r="B27" s="26">
         <f>TEXT(B11,"0.000")</f>
         <v/>
       </c>
-      <c r="C27" s="27" t="inlineStr">
+      <c r="C27" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; airplane efficiency factor</t>
         </is>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="27" t="inlineStr">
+      <c r="A28" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :TAF</t>
         </is>
       </c>
-      <c r="B28" s="27">
+      <c r="B28" s="26">
         <f>TEXT(B12,"0.0")</f>
         <v/>
       </c>
-      <c r="C28" s="27" t="inlineStr">
+      <c r="C28" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; total activity factor</t>
         </is>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="27" t="inlineStr">
+      <c r="A29" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :Z</t>
         </is>
       </c>
-      <c r="B29" s="27">
+      <c r="B29" s="26">
         <f>TEXT(B13,"0.000")</f>
         <v/>
       </c>
-      <c r="C29" s="27" t="inlineStr">
+      <c r="C29" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; fuselage dia / prop dia</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="27" t="inlineStr">
+      <c r="A30" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :tractor?</t>
         </is>
       </c>
-      <c r="B30" s="27">
+      <c r="B30" s="26">
         <f>IF(B14=1,"true","false")</f>
         <v/>
       </c>
-      <c r="C30" s="27" t="inlineStr"/>
+      <c r="C30" s="26" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="27" t="inlineStr">
+      <c r="A31" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :BB</t>
         </is>
       </c>
-      <c r="B31" s="27">
+      <c r="B31" s="26">
         <f>TEXT(B15,"0")</f>
         <v/>
       </c>
-      <c r="C31" s="27" t="inlineStr">
+      <c r="C31" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve">  ;; number of blades</t>
         </is>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="27" t="inlineStr">
+      <c r="A32" s="26" t="inlineStr">
         <is>
           <t xml:space="preserve"> :C</t>
         </is>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="26">
         <f>TEXT(B16,"0.00")</f>
         <v/>
       </c>
-      <c r="C32" s="27" t="inlineStr">
+      <c r="C32" s="26" t="inlineStr">
         <is>
           <t>}  ;; altitude power dropoff</t>
         </is>
@@ -4054,28 +3998,28 @@
           <t>(constant)</t>
         </is>
       </c>
-      <c r="C6" s="28" t="n">
+      <c r="C6" s="27" t="n">
         <v>-0.027280541925</v>
       </c>
-      <c r="D6" s="28" t="n">
+      <c r="D6" s="27" t="n">
         <v>-0.038502996895</v>
       </c>
-      <c r="E6" s="28" t="n">
+      <c r="E6" s="27" t="n">
         <v>-0.026741905</v>
       </c>
-      <c r="F6" s="28" t="n">
+      <c r="F6" s="27" t="n">
         <v>0.038100252152</v>
       </c>
-      <c r="G6" s="28" t="n">
+      <c r="G6" s="27" t="n">
         <v>0.251897476</v>
       </c>
-      <c r="H6" s="28" t="n">
+      <c r="H6" s="27" t="n">
         <v>0.140144145675</v>
       </c>
-      <c r="I6" s="28" t="n">
+      <c r="I6" s="27" t="n">
         <v>-0.70560405</v>
       </c>
-      <c r="J6" s="28" t="n">
+      <c r="J6" s="27" t="n">
         <v>-2.340532183939</v>
       </c>
     </row>
@@ -4090,28 +4034,28 @@
           <t>(h)</t>
         </is>
       </c>
-      <c r="C7" s="28" t="n">
+      <c r="C7" s="27" t="n">
         <v>1.157818942224</v>
       </c>
-      <c r="D7" s="28" t="n">
+      <c r="D7" s="27" t="n">
         <v>1.046135815788</v>
       </c>
-      <c r="E7" s="28" t="n">
+      <c r="E7" s="27" t="n">
         <v>0.7175824135</v>
       </c>
-      <c r="F7" s="28" t="n">
+      <c r="F7" s="27" t="n">
         <v>0.19952245559</v>
       </c>
-      <c r="G7" s="28" t="n">
+      <c r="G7" s="27" t="n">
         <v>-0.56166584</v>
       </c>
-      <c r="H7" s="28" t="n">
+      <c r="H7" s="27" t="n">
         <v>0.071636129794</v>
       </c>
-      <c r="I7" s="28" t="n">
+      <c r="I7" s="27" t="n">
         <v>2.868232531</v>
       </c>
-      <c r="J7" s="28" t="n">
+      <c r="J7" s="27" t="n">
         <v>7.56393789715</v>
       </c>
     </row>
@@ -4126,28 +4070,28 @@
           <t>(h²)</t>
         </is>
       </c>
-      <c r="C8" s="28" t="n">
+      <c r="C8" s="27" t="n">
         <v>-0.5489231230129999</v>
       </c>
-      <c r="D8" s="28" t="n">
+      <c r="D8" s="27" t="n">
         <v>-0.485313329667</v>
       </c>
-      <c r="E8" s="28" t="n">
+      <c r="E8" s="27" t="n">
         <v>-0.08467334999999999</v>
       </c>
-      <c r="F8" s="28" t="n">
+      <c r="F8" s="27" t="n">
         <v>0.458898025445</v>
       </c>
-      <c r="G8" s="28" t="n">
+      <c r="G8" s="27" t="n">
         <v>1.13905513</v>
       </c>
-      <c r="H8" s="28" t="n">
+      <c r="H8" s="27" t="n">
         <v>-0.057356417627</v>
       </c>
-      <c r="I8" s="28" t="n">
+      <c r="I8" s="27" t="n">
         <v>-3.651371295</v>
       </c>
-      <c r="J8" s="28" t="n">
+      <c r="J8" s="27" t="n">
         <v>-9.020964992474999</v>
       </c>
     </row>
@@ -4162,28 +4106,28 @@
           <t>(h³)</t>
         </is>
       </c>
-      <c r="C9" s="28" t="n">
+      <c r="C9" s="27" t="n">
         <v>0.038551650269</v>
       </c>
-      <c r="D9" s="28" t="n">
+      <c r="D9" s="27" t="n">
         <v>0.130100232509</v>
       </c>
-      <c r="E9" s="28" t="n">
+      <c r="E9" s="27" t="n">
         <v>-0.07445168000000001</v>
       </c>
-      <c r="F9" s="28" t="n">
+      <c r="F9" s="27" t="n">
         <v>-0.318992736679</v>
       </c>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="27" t="n">
         <v>-0.60219333</v>
       </c>
-      <c r="H9" s="28" t="n">
+      <c r="H9" s="27" t="n">
         <v>0.276378945894</v>
       </c>
-      <c r="I9" s="28" t="n">
+      <c r="I9" s="27" t="n">
         <v>2.487262933</v>
       </c>
-      <c r="J9" s="28" t="n">
+      <c r="J9" s="27" t="n">
         <v>5.550045133294</v>
       </c>
     </row>
@@ -4198,28 +4142,28 @@
           <t>(h⁴)</t>
         </is>
       </c>
-      <c r="C10" s="28" t="n">
+      <c r="C10" s="27" t="n">
         <v>0.06458055527999999</v>
       </c>
-      <c r="D10" s="28" t="n">
+      <c r="D10" s="27" t="n">
         <v>-0.027326610124</v>
       </c>
-      <c r="E10" s="28" t="n">
+      <c r="E10" s="27" t="n">
         <v>0.026437051</v>
       </c>
-      <c r="F10" s="28" t="n">
+      <c r="F10" s="27" t="n">
         <v>0.081357821405</v>
       </c>
-      <c r="G10" s="28" t="n">
+      <c r="G10" s="27" t="n">
         <v>0.144341736</v>
       </c>
-      <c r="H10" s="28" t="n">
+      <c r="H10" s="27" t="n">
         <v>-0.159843307011</v>
       </c>
-      <c r="I10" s="28" t="n">
+      <c r="I10" s="27" t="n">
         <v>-0.8634212</v>
       </c>
-      <c r="J10" s="28" t="n">
+      <c r="J10" s="27" t="n">
         <v>-1.793776917489</v>
       </c>
     </row>
@@ -4234,28 +4178,28 @@
           <t>(h⁵)</t>
         </is>
       </c>
-      <c r="C11" s="28" t="n">
+      <c r="C11" s="27" t="n">
         <v>-0.026301243311</v>
       </c>
-      <c r="D11" s="28" t="n">
+      <c r="D11" s="27" t="n">
         <v>0.003139013961</v>
       </c>
-      <c r="E11" s="28" t="n">
+      <c r="E11" s="27" t="n">
         <v>-0.003537565</v>
       </c>
-      <c r="F11" s="28" t="n">
+      <c r="F11" s="27" t="n">
         <v>-0.009083801712</v>
       </c>
-      <c r="G11" s="28" t="n">
+      <c r="G11" s="27" t="n">
         <v>-0.01619473</v>
       </c>
-      <c r="H11" s="28" t="n">
+      <c r="H11" s="27" t="n">
         <v>0.034239846258</v>
       </c>
-      <c r="I11" s="28" t="n">
+      <c r="I11" s="27" t="n">
         <v>0.1464783315</v>
       </c>
-      <c r="J11" s="28" t="n">
+      <c r="J11" s="27" t="n">
         <v>0.291020480454</v>
       </c>
     </row>
@@ -4270,28 +4214,28 @@
           <t>(h⁶)</t>
         </is>
       </c>
-      <c r="C12" s="28" t="n">
+      <c r="C12" s="27" t="n">
         <v>0.003017419881</v>
       </c>
-      <c r="D12" s="28" t="n">
+      <c r="D12" s="27" t="n">
         <v>-0.000131566345</v>
       </c>
-      <c r="E12" s="28" t="n">
+      <c r="E12" s="27" t="n">
         <v>0.000177733</v>
       </c>
-      <c r="F12" s="28" t="n">
+      <c r="F12" s="27" t="n">
         <v>0.000350613126</v>
       </c>
-      <c r="G12" s="28" t="n">
+      <c r="G12" s="27" t="n">
         <v>0.000664038</v>
       </c>
-      <c r="H12" s="28" t="n">
+      <c r="H12" s="27" t="n">
         <v>-0.002573002786</v>
       </c>
-      <c r="I12" s="28" t="n">
+      <c r="I12" s="27" t="n">
         <v>-0.009686854999999999</v>
       </c>
-      <c r="J12" s="28" t="n">
+      <c r="J12" s="27" t="n">
         <v>-0.018743169313</v>
       </c>
     </row>
@@ -4411,7 +4355,7 @@
           <t>N0 (rated RPM)</t>
         </is>
       </c>
-      <c r="B22" s="29">
+      <c r="B22" s="28">
         <f>'Data Plate'!B8</f>
         <v/>
       </c>
@@ -4487,7 +4431,7 @@
           <t>Tractor? (1=yes, 0=no)</t>
         </is>
       </c>
-      <c r="B28" s="29">
+      <c r="B28" s="28">
         <f>'Data Plate'!B14</f>
         <v/>
       </c>
@@ -4498,7 +4442,7 @@
           <t>BB (num blades)</t>
         </is>
       </c>
-      <c r="B29" s="29">
+      <c r="B29" s="28">
         <f>'Data Plate'!B15</f>
         <v/>
       </c>
@@ -4532,7 +4476,7 @@
           <t>W (gross weight)</t>
         </is>
       </c>
-      <c r="B33" s="30" t="n">
+      <c r="B33" s="29" t="n">
         <v>3100</v>
       </c>
       <c r="C33" t="inlineStr">
@@ -4547,7 +4491,7 @@
           <t>h (density alt)</t>
         </is>
       </c>
-      <c r="B34" s="31" t="n">
+      <c r="B34" s="30" t="n">
         <v>8000</v>
       </c>
       <c r="C34" t="inlineStr">
@@ -4562,7 +4506,7 @@
           <t>N (RPM)</t>
         </is>
       </c>
-      <c r="B35" s="31" t="n">
+      <c r="B35" s="30" t="n">
         <v>2300</v>
       </c>
     </row>
@@ -4572,7 +4516,7 @@
           <t>% Power (0–1)</t>
         </is>
       </c>
-      <c r="B36" s="26" t="n">
+      <c r="B36" s="25" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -4744,7 +4688,7 @@
           <t>GAGPC bracket idx</t>
         </is>
       </c>
-      <c r="B49" s="32">
+      <c r="B49" s="31">
         <f>MIN(MATCH(B48,$C$5:$J$5,1),7)</f>
         <v/>
       </c>
@@ -4957,7 +4901,7 @@
           <t>σ</t>
         </is>
       </c>
-      <c r="B64" s="33" t="n">
+      <c r="B64" s="32" t="n">
         <v>0.786</v>
       </c>
       <c r="C64" s="15">
@@ -4975,7 +4919,7 @@
           <t>ρ</t>
         </is>
       </c>
-      <c r="B65" s="34" t="n">
+      <c r="B65" s="33" t="n">
         <v>0.001868</v>
       </c>
       <c r="C65" s="20">
@@ -4993,7 +4937,7 @@
           <t>φ</t>
         </is>
       </c>
-      <c r="B66" s="33" t="n">
+      <c r="B66" s="32" t="n">
         <v>0.7568</v>
       </c>
       <c r="C66" s="15">
@@ -5011,7 +4955,7 @@
           <t>X</t>
         </is>
       </c>
-      <c r="B67" s="33" t="n">
+      <c r="B67" s="32" t="n">
         <v>0.2088</v>
       </c>
       <c r="C67" s="15">
@@ -5029,7 +4973,7 @@
           <t>SDF</t>
         </is>
       </c>
-      <c r="B68" s="35" t="n">
+      <c r="B68" s="34" t="n">
         <v>0.91</v>
       </c>
       <c r="C68" s="18">
@@ -5059,7 +5003,7 @@
           <t>η (eta)</t>
         </is>
       </c>
-      <c r="B71" s="35" t="n">
+      <c r="B71" s="34" t="n">
         <v>0.617</v>
       </c>
       <c r="C71" s="18">
@@ -5149,7 +5093,7 @@
           <t>ROC</t>
         </is>
       </c>
-      <c r="B76" s="36" t="n">
+      <c r="B76" s="35" t="n">
         <v>273.23</v>
       </c>
       <c r="C76" s="19">
@@ -5167,7 +5111,7 @@
           <t>ROS</t>
         </is>
       </c>
-      <c r="B77" s="36" t="n">
+      <c r="B77" s="35" t="n">
         <v>729.37</v>
       </c>
       <c r="C77" s="19">
@@ -5185,7 +5129,7 @@
           <t>AOG</t>
         </is>
       </c>
-      <c r="B78" s="35" t="n">
+      <c r="B78" s="34" t="n">
         <v>6.109</v>
       </c>
       <c r="C78" s="18">
@@ -5210,7 +5154,7 @@
           <t>Vy KCAS</t>
         </is>
       </c>
-      <c r="B81" s="36" t="n">
+      <c r="B81" s="35" t="n">
         <v>77</v>
       </c>
       <c r="C81" s="19">
@@ -5228,7 +5172,7 @@
           <t>Vy ROC</t>
         </is>
       </c>
-      <c r="B82" s="36" t="n">
+      <c r="B82" s="35" t="n">
         <v>371.7</v>
       </c>
       <c r="C82" s="19">
@@ -5246,7 +5190,7 @@
           <t>Vx KCAS</t>
         </is>
       </c>
-      <c r="B83" s="36" t="n">
+      <c r="B83" s="35" t="n">
         <v>69.5</v>
       </c>
       <c r="C83" s="19">
@@ -5282,7 +5226,7 @@
           <t>Vbg KCAS</t>
         </is>
       </c>
-      <c r="B85" s="36" t="n">
+      <c r="B85" s="35" t="n">
         <v>87</v>
       </c>
       <c r="C85" s="19">
@@ -5318,7 +5262,7 @@
           <t>Vmd KCAS</t>
         </is>
       </c>
-      <c r="B87" s="36" t="n">
+      <c r="B87" s="35" t="n">
         <v>66</v>
       </c>
       <c r="C87" s="19">
@@ -5336,7 +5280,7 @@
           <t>Vmd ROS</t>
         </is>
       </c>
-      <c r="B88" s="36" t="n">
+      <c r="B88" s="35" t="n">
         <v>719.9</v>
       </c>
       <c r="C88" s="19">
@@ -5354,7 +5298,7 @@
           <t>VM KCAS</t>
         </is>
       </c>
-      <c r="B89" s="36" t="n">
+      <c r="B89" s="35" t="n">
         <v>111.5</v>
       </c>
       <c r="C89" s="19">
@@ -5473,7 +5417,7 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="36" t="n">
+      <c r="A95" s="35" t="n">
         <v>60</v>
       </c>
       <c r="B95" s="19">
@@ -5542,7 +5486,7 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="36" t="n">
+      <c r="A96" s="35" t="n">
         <v>60.5</v>
       </c>
       <c r="B96" s="19">
@@ -5611,7 +5555,7 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="36" t="n">
+      <c r="A97" s="35" t="n">
         <v>61</v>
       </c>
       <c r="B97" s="19">
@@ -5680,7 +5624,7 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="36" t="n">
+      <c r="A98" s="35" t="n">
         <v>61.5</v>
       </c>
       <c r="B98" s="19">
@@ -5749,7 +5693,7 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="36" t="n">
+      <c r="A99" s="35" t="n">
         <v>62</v>
       </c>
       <c r="B99" s="19">
@@ -5818,7 +5762,7 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="36" t="n">
+      <c r="A100" s="35" t="n">
         <v>62.5</v>
       </c>
       <c r="B100" s="19">
@@ -5887,7 +5831,7 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="36" t="n">
+      <c r="A101" s="35" t="n">
         <v>63</v>
       </c>
       <c r="B101" s="19">
@@ -5956,7 +5900,7 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="36" t="n">
+      <c r="A102" s="35" t="n">
         <v>63.5</v>
       </c>
       <c r="B102" s="19">
@@ -6025,7 +5969,7 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="36" t="n">
+      <c r="A103" s="35" t="n">
         <v>64</v>
       </c>
       <c r="B103" s="19">
@@ -6094,7 +6038,7 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="36" t="n">
+      <c r="A104" s="35" t="n">
         <v>64.5</v>
       </c>
       <c r="B104" s="19">
@@ -6163,7 +6107,7 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="36" t="n">
+      <c r="A105" s="35" t="n">
         <v>65</v>
       </c>
       <c r="B105" s="19">
@@ -6232,7 +6176,7 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="36" t="n">
+      <c r="A106" s="35" t="n">
         <v>65.5</v>
       </c>
       <c r="B106" s="19">
@@ -6301,7 +6245,7 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="36" t="n">
+      <c r="A107" s="35" t="n">
         <v>66</v>
       </c>
       <c r="B107" s="19">
@@ -6370,7 +6314,7 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="36" t="n">
+      <c r="A108" s="35" t="n">
         <v>66.5</v>
       </c>
       <c r="B108" s="19">
@@ -6439,7 +6383,7 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="36" t="n">
+      <c r="A109" s="35" t="n">
         <v>67</v>
       </c>
       <c r="B109" s="19">
@@ -6508,7 +6452,7 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="36" t="n">
+      <c r="A110" s="35" t="n">
         <v>67.5</v>
       </c>
       <c r="B110" s="19">
@@ -6577,7 +6521,7 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="36" t="n">
+      <c r="A111" s="35" t="n">
         <v>68</v>
       </c>
       <c r="B111" s="19">
@@ -6646,7 +6590,7 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="36" t="n">
+      <c r="A112" s="35" t="n">
         <v>68.5</v>
       </c>
       <c r="B112" s="19">
@@ -6715,7 +6659,7 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="36" t="n">
+      <c r="A113" s="35" t="n">
         <v>69</v>
       </c>
       <c r="B113" s="19">
@@ -6784,7 +6728,7 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="36" t="n">
+      <c r="A114" s="35" t="n">
         <v>69.5</v>
       </c>
       <c r="B114" s="19">
@@ -6853,7 +6797,7 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="36" t="n">
+      <c r="A115" s="35" t="n">
         <v>70</v>
       </c>
       <c r="B115" s="19">
@@ -6922,7 +6866,7 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="36" t="n">
+      <c r="A116" s="35" t="n">
         <v>70.5</v>
       </c>
       <c r="B116" s="19">
@@ -6991,7 +6935,7 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="36" t="n">
+      <c r="A117" s="35" t="n">
         <v>71</v>
       </c>
       <c r="B117" s="19">
@@ -7060,7 +7004,7 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="36" t="n">
+      <c r="A118" s="35" t="n">
         <v>71.5</v>
       </c>
       <c r="B118" s="19">
@@ -7129,7 +7073,7 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="36" t="n">
+      <c r="A119" s="35" t="n">
         <v>72</v>
       </c>
       <c r="B119" s="19">
@@ -7198,7 +7142,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="36" t="n">
+      <c r="A120" s="35" t="n">
         <v>72.5</v>
       </c>
       <c r="B120" s="19">
@@ -7267,7 +7211,7 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="36" t="n">
+      <c r="A121" s="35" t="n">
         <v>73</v>
       </c>
       <c r="B121" s="19">
@@ -7336,7 +7280,7 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="36" t="n">
+      <c r="A122" s="35" t="n">
         <v>73.5</v>
       </c>
       <c r="B122" s="19">
@@ -7405,7 +7349,7 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="36" t="n">
+      <c r="A123" s="35" t="n">
         <v>74</v>
       </c>
       <c r="B123" s="19">
@@ -7474,7 +7418,7 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="36" t="n">
+      <c r="A124" s="35" t="n">
         <v>74.5</v>
       </c>
       <c r="B124" s="19">
@@ -7543,7 +7487,7 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="36" t="n">
+      <c r="A125" s="35" t="n">
         <v>75</v>
       </c>
       <c r="B125" s="19">
@@ -7612,7 +7556,7 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="36" t="n">
+      <c r="A126" s="35" t="n">
         <v>75.5</v>
       </c>
       <c r="B126" s="19">
@@ -7681,7 +7625,7 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="36" t="n">
+      <c r="A127" s="35" t="n">
         <v>76</v>
       </c>
       <c r="B127" s="19">
@@ -7750,7 +7694,7 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="36" t="n">
+      <c r="A128" s="35" t="n">
         <v>76.5</v>
       </c>
       <c r="B128" s="19">
@@ -7819,7 +7763,7 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="36" t="n">
+      <c r="A129" s="35" t="n">
         <v>77</v>
       </c>
       <c r="B129" s="19">
@@ -7888,7 +7832,7 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="36" t="n">
+      <c r="A130" s="35" t="n">
         <v>77.5</v>
       </c>
       <c r="B130" s="19">
@@ -7957,7 +7901,7 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="36" t="n">
+      <c r="A131" s="35" t="n">
         <v>78</v>
       </c>
       <c r="B131" s="19">
@@ -8026,7 +7970,7 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="36" t="n">
+      <c r="A132" s="35" t="n">
         <v>78.5</v>
       </c>
       <c r="B132" s="19">
@@ -8095,7 +8039,7 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="36" t="n">
+      <c r="A133" s="35" t="n">
         <v>79</v>
       </c>
       <c r="B133" s="19">
@@ -8164,7 +8108,7 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="36" t="n">
+      <c r="A134" s="35" t="n">
         <v>79.5</v>
       </c>
       <c r="B134" s="19">
@@ -8233,7 +8177,7 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="36" t="n">
+      <c r="A135" s="35" t="n">
         <v>80</v>
       </c>
       <c r="B135" s="19">
@@ -8302,7 +8246,7 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="36" t="n">
+      <c r="A136" s="35" t="n">
         <v>80.5</v>
       </c>
       <c r="B136" s="19">
@@ -8371,7 +8315,7 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="36" t="n">
+      <c r="A137" s="35" t="n">
         <v>81</v>
       </c>
       <c r="B137" s="19">
@@ -8440,7 +8384,7 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="36" t="n">
+      <c r="A138" s="35" t="n">
         <v>81.5</v>
       </c>
       <c r="B138" s="19">
@@ -8509,7 +8453,7 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="36" t="n">
+      <c r="A139" s="35" t="n">
         <v>82</v>
       </c>
       <c r="B139" s="19">
@@ -8578,7 +8522,7 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="36" t="n">
+      <c r="A140" s="35" t="n">
         <v>82.5</v>
       </c>
       <c r="B140" s="19">
@@ -8647,7 +8591,7 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="36" t="n">
+      <c r="A141" s="35" t="n">
         <v>83</v>
       </c>
       <c r="B141" s="19">
@@ -8716,7 +8660,7 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="36" t="n">
+      <c r="A142" s="35" t="n">
         <v>83.5</v>
       </c>
       <c r="B142" s="19">
@@ -8785,7 +8729,7 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="36" t="n">
+      <c r="A143" s="35" t="n">
         <v>84</v>
       </c>
       <c r="B143" s="19">
@@ -8854,7 +8798,7 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="36" t="n">
+      <c r="A144" s="35" t="n">
         <v>84.5</v>
       </c>
       <c r="B144" s="19">
@@ -8923,7 +8867,7 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="36" t="n">
+      <c r="A145" s="35" t="n">
         <v>85</v>
       </c>
       <c r="B145" s="19">
@@ -8992,7 +8936,7 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="36" t="n">
+      <c r="A146" s="35" t="n">
         <v>85.5</v>
       </c>
       <c r="B146" s="19">
@@ -9061,7 +9005,7 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="36" t="n">
+      <c r="A147" s="35" t="n">
         <v>86</v>
       </c>
       <c r="B147" s="19">
@@ -9130,7 +9074,7 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="36" t="n">
+      <c r="A148" s="35" t="n">
         <v>86.5</v>
       </c>
       <c r="B148" s="19">
@@ -9199,7 +9143,7 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="36" t="n">
+      <c r="A149" s="35" t="n">
         <v>87</v>
       </c>
       <c r="B149" s="19">
@@ -9268,7 +9212,7 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="36" t="n">
+      <c r="A150" s="35" t="n">
         <v>87.5</v>
       </c>
       <c r="B150" s="19">
@@ -9337,7 +9281,7 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="36" t="n">
+      <c r="A151" s="35" t="n">
         <v>88</v>
       </c>
       <c r="B151" s="19">
@@ -9406,7 +9350,7 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="36" t="n">
+      <c r="A152" s="35" t="n">
         <v>88.5</v>
       </c>
       <c r="B152" s="19">
@@ -9475,7 +9419,7 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="36" t="n">
+      <c r="A153" s="35" t="n">
         <v>89</v>
       </c>
       <c r="B153" s="19">
@@ -9544,7 +9488,7 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="36" t="n">
+      <c r="A154" s="35" t="n">
         <v>89.5</v>
       </c>
       <c r="B154" s="19">
@@ -9613,7 +9557,7 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="36" t="n">
+      <c r="A155" s="35" t="n">
         <v>90</v>
       </c>
       <c r="B155" s="19">
@@ -9682,7 +9626,7 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="36" t="n">
+      <c r="A156" s="35" t="n">
         <v>90.5</v>
       </c>
       <c r="B156" s="19">
@@ -9751,7 +9695,7 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="36" t="n">
+      <c r="A157" s="35" t="n">
         <v>91</v>
       </c>
       <c r="B157" s="19">
@@ -9820,7 +9764,7 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="36" t="n">
+      <c r="A158" s="35" t="n">
         <v>91.5</v>
       </c>
       <c r="B158" s="19">
@@ -9889,7 +9833,7 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="36" t="n">
+      <c r="A159" s="35" t="n">
         <v>92</v>
       </c>
       <c r="B159" s="19">
@@ -9958,7 +9902,7 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="36" t="n">
+      <c r="A160" s="35" t="n">
         <v>92.5</v>
       </c>
       <c r="B160" s="19">
@@ -10027,7 +9971,7 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="36" t="n">
+      <c r="A161" s="35" t="n">
         <v>93</v>
       </c>
       <c r="B161" s="19">
@@ -10096,7 +10040,7 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="36" t="n">
+      <c r="A162" s="35" t="n">
         <v>93.5</v>
       </c>
       <c r="B162" s="19">
@@ -10165,7 +10109,7 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="36" t="n">
+      <c r="A163" s="35" t="n">
         <v>94</v>
       </c>
       <c r="B163" s="19">
@@ -10234,7 +10178,7 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="36" t="n">
+      <c r="A164" s="35" t="n">
         <v>94.5</v>
       </c>
       <c r="B164" s="19">
@@ -10303,7 +10247,7 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="36" t="n">
+      <c r="A165" s="35" t="n">
         <v>95</v>
       </c>
       <c r="B165" s="19">
@@ -10372,7 +10316,7 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="36" t="n">
+      <c r="A166" s="35" t="n">
         <v>95.5</v>
       </c>
       <c r="B166" s="19">
@@ -10441,7 +10385,7 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="36" t="n">
+      <c r="A167" s="35" t="n">
         <v>96</v>
       </c>
       <c r="B167" s="19">
@@ -10510,7 +10454,7 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="36" t="n">
+      <c r="A168" s="35" t="n">
         <v>96.5</v>
       </c>
       <c r="B168" s="19">
@@ -10579,7 +10523,7 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="36" t="n">
+      <c r="A169" s="35" t="n">
         <v>97</v>
       </c>
       <c r="B169" s="19">
@@ -10648,7 +10592,7 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="36" t="n">
+      <c r="A170" s="35" t="n">
         <v>97.5</v>
       </c>
       <c r="B170" s="19">
@@ -10717,7 +10661,7 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="36" t="n">
+      <c r="A171" s="35" t="n">
         <v>98</v>
       </c>
       <c r="B171" s="19">
@@ -10786,7 +10730,7 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="36" t="n">
+      <c r="A172" s="35" t="n">
         <v>98.5</v>
       </c>
       <c r="B172" s="19">
@@ -10855,7 +10799,7 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="36" t="n">
+      <c r="A173" s="35" t="n">
         <v>99</v>
       </c>
       <c r="B173" s="19">
@@ -10924,7 +10868,7 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="36" t="n">
+      <c r="A174" s="35" t="n">
         <v>99.5</v>
       </c>
       <c r="B174" s="19">
@@ -10993,7 +10937,7 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="36" t="n">
+      <c r="A175" s="35" t="n">
         <v>100</v>
       </c>
       <c r="B175" s="19">
@@ -11062,7 +11006,7 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="36" t="n">
+      <c r="A176" s="35" t="n">
         <v>100.5</v>
       </c>
       <c r="B176" s="19">
@@ -11131,7 +11075,7 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="36" t="n">
+      <c r="A177" s="35" t="n">
         <v>101</v>
       </c>
       <c r="B177" s="19">
@@ -11200,7 +11144,7 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="36" t="n">
+      <c r="A178" s="35" t="n">
         <v>101.5</v>
       </c>
       <c r="B178" s="19">
@@ -11269,7 +11213,7 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="36" t="n">
+      <c r="A179" s="35" t="n">
         <v>102</v>
       </c>
       <c r="B179" s="19">
@@ -11338,7 +11282,7 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="36" t="n">
+      <c r="A180" s="35" t="n">
         <v>102.5</v>
       </c>
       <c r="B180" s="19">
@@ -11407,7 +11351,7 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="36" t="n">
+      <c r="A181" s="35" t="n">
         <v>103</v>
       </c>
       <c r="B181" s="19">
@@ -11476,7 +11420,7 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="36" t="n">
+      <c r="A182" s="35" t="n">
         <v>103.5</v>
       </c>
       <c r="B182" s="19">
@@ -11545,7 +11489,7 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="36" t="n">
+      <c r="A183" s="35" t="n">
         <v>104</v>
       </c>
       <c r="B183" s="19">
@@ -11614,7 +11558,7 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="36" t="n">
+      <c r="A184" s="35" t="n">
         <v>104.5</v>
       </c>
       <c r="B184" s="19">
@@ -11683,7 +11627,7 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="36" t="n">
+      <c r="A185" s="35" t="n">
         <v>105</v>
       </c>
       <c r="B185" s="19">
@@ -11752,7 +11696,7 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="36" t="n">
+      <c r="A186" s="35" t="n">
         <v>105.5</v>
       </c>
       <c r="B186" s="19">
@@ -11821,7 +11765,7 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="36" t="n">
+      <c r="A187" s="35" t="n">
         <v>106</v>
       </c>
       <c r="B187" s="19">
@@ -11890,7 +11834,7 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="36" t="n">
+      <c r="A188" s="35" t="n">
         <v>106.5</v>
       </c>
       <c r="B188" s="19">
@@ -11959,7 +11903,7 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="36" t="n">
+      <c r="A189" s="35" t="n">
         <v>107</v>
       </c>
       <c r="B189" s="19">
@@ -12028,7 +11972,7 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="36" t="n">
+      <c r="A190" s="35" t="n">
         <v>107.5</v>
       </c>
       <c r="B190" s="19">
@@ -12097,7 +12041,7 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="36" t="n">
+      <c r="A191" s="35" t="n">
         <v>108</v>
       </c>
       <c r="B191" s="19">
@@ -12166,7 +12110,7 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="36" t="n">
+      <c r="A192" s="35" t="n">
         <v>108.5</v>
       </c>
       <c r="B192" s="19">
@@ -12235,7 +12179,7 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="36" t="n">
+      <c r="A193" s="35" t="n">
         <v>109</v>
       </c>
       <c r="B193" s="19">
@@ -12304,7 +12248,7 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="36" t="n">
+      <c r="A194" s="35" t="n">
         <v>109.5</v>
       </c>
       <c r="B194" s="19">
@@ -12373,7 +12317,7 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="36" t="n">
+      <c r="A195" s="35" t="n">
         <v>110</v>
       </c>
       <c r="B195" s="19">
@@ -12442,7 +12386,7 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="36" t="n">
+      <c r="A196" s="35" t="n">
         <v>110.5</v>
       </c>
       <c r="B196" s="19">
@@ -12511,7 +12455,7 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="36" t="n">
+      <c r="A197" s="35" t="n">
         <v>111</v>
       </c>
       <c r="B197" s="19">
@@ -12580,7 +12524,7 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="36" t="n">
+      <c r="A198" s="35" t="n">
         <v>111.5</v>
       </c>
       <c r="B198" s="19">
@@ -12649,7 +12593,7 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="36" t="n">
+      <c r="A199" s="35" t="n">
         <v>112</v>
       </c>
       <c r="B199" s="19">
@@ -12718,7 +12662,7 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="36" t="n">
+      <c r="A200" s="35" t="n">
         <v>112.5</v>
       </c>
       <c r="B200" s="19">
@@ -12787,7 +12731,7 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="36" t="n">
+      <c r="A201" s="35" t="n">
         <v>113</v>
       </c>
       <c r="B201" s="19">
@@ -12856,7 +12800,7 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="36" t="n">
+      <c r="A202" s="35" t="n">
         <v>113.5</v>
       </c>
       <c r="B202" s="19">
@@ -12925,7 +12869,7 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="36" t="n">
+      <c r="A203" s="35" t="n">
         <v>114</v>
       </c>
       <c r="B203" s="19">
@@ -12994,7 +12938,7 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="36" t="n">
+      <c r="A204" s="35" t="n">
         <v>114.5</v>
       </c>
       <c r="B204" s="19">
@@ -13063,7 +13007,7 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="36" t="n">
+      <c r="A205" s="35" t="n">
         <v>115</v>
       </c>
       <c r="B205" s="19">
@@ -13132,7 +13076,7 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="36" t="n">
+      <c r="A206" s="35" t="n">
         <v>115.5</v>
       </c>
       <c r="B206" s="19">
@@ -13201,7 +13145,7 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="36" t="n">
+      <c r="A207" s="35" t="n">
         <v>116</v>
       </c>
       <c r="B207" s="19">
@@ -13270,7 +13214,7 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="36" t="n">
+      <c r="A208" s="35" t="n">
         <v>116.5</v>
       </c>
       <c r="B208" s="19">
@@ -13339,7 +13283,7 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="36" t="n">
+      <c r="A209" s="35" t="n">
         <v>117</v>
       </c>
       <c r="B209" s="19">
@@ -13408,7 +13352,7 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="36" t="n">
+      <c r="A210" s="35" t="n">
         <v>117.5</v>
       </c>
       <c r="B210" s="19">
@@ -13477,7 +13421,7 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="36" t="n">
+      <c r="A211" s="35" t="n">
         <v>118</v>
       </c>
       <c r="B211" s="19">
@@ -13546,7 +13490,7 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="36" t="n">
+      <c r="A212" s="35" t="n">
         <v>118.5</v>
       </c>
       <c r="B212" s="19">
@@ -13615,7 +13559,7 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="36" t="n">
+      <c r="A213" s="35" t="n">
         <v>119</v>
       </c>
       <c r="B213" s="19">
@@ -13684,7 +13628,7 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="36" t="n">
+      <c r="A214" s="35" t="n">
         <v>119.5</v>
       </c>
       <c r="B214" s="19">
@@ -13753,7 +13697,7 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="36" t="n">
+      <c r="A215" s="35" t="n">
         <v>120</v>
       </c>
       <c r="B215" s="19">
@@ -13822,7 +13766,7 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="36" t="n">
+      <c r="A216" s="35" t="n">
         <v>120.5</v>
       </c>
       <c r="B216" s="19">
@@ -13891,7 +13835,7 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="36" t="n">
+      <c r="A217" s="35" t="n">
         <v>121</v>
       </c>
       <c r="B217" s="19">
@@ -13960,7 +13904,7 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="36" t="n">
+      <c r="A218" s="35" t="n">
         <v>121.5</v>
       </c>
       <c r="B218" s="19">
@@ -14029,7 +13973,7 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="36" t="n">
+      <c r="A219" s="35" t="n">
         <v>122</v>
       </c>
       <c r="B219" s="19">
@@ -14098,7 +14042,7 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="36" t="n">
+      <c r="A220" s="35" t="n">
         <v>122.5</v>
       </c>
       <c r="B220" s="19">
@@ -14167,7 +14111,7 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="36" t="n">
+      <c r="A221" s="35" t="n">
         <v>123</v>
       </c>
       <c r="B221" s="19">
@@ -14236,7 +14180,7 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="36" t="n">
+      <c r="A222" s="35" t="n">
         <v>123.5</v>
       </c>
       <c r="B222" s="19">
@@ -14305,7 +14249,7 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="36" t="n">
+      <c r="A223" s="35" t="n">
         <v>124</v>
       </c>
       <c r="B223" s="19">
@@ -14374,7 +14318,7 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="36" t="n">
+      <c r="A224" s="35" t="n">
         <v>124.5</v>
       </c>
       <c r="B224" s="19">
@@ -14443,7 +14387,7 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="36" t="n">
+      <c r="A225" s="35" t="n">
         <v>125</v>
       </c>
       <c r="B225" s="19">
@@ -14512,7 +14456,7 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="36" t="n">
+      <c r="A226" s="35" t="n">
         <v>125.5</v>
       </c>
       <c r="B226" s="19">
@@ -14581,7 +14525,7 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="36" t="n">
+      <c r="A227" s="35" t="n">
         <v>126</v>
       </c>
       <c r="B227" s="19">
@@ -14650,7 +14594,7 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="36" t="n">
+      <c r="A228" s="35" t="n">
         <v>126.5</v>
       </c>
       <c r="B228" s="19">
@@ -14719,7 +14663,7 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="36" t="n">
+      <c r="A229" s="35" t="n">
         <v>127</v>
       </c>
       <c r="B229" s="19">
@@ -14788,7 +14732,7 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="36" t="n">
+      <c r="A230" s="35" t="n">
         <v>127.5</v>
       </c>
       <c r="B230" s="19">
@@ -14857,7 +14801,7 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="36" t="n">
+      <c r="A231" s="35" t="n">
         <v>128</v>
       </c>
       <c r="B231" s="19">
@@ -14926,7 +14870,7 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="36" t="n">
+      <c r="A232" s="35" t="n">
         <v>128.5</v>
       </c>
       <c r="B232" s="19">
@@ -14995,7 +14939,7 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="36" t="n">
+      <c r="A233" s="35" t="n">
         <v>129</v>
       </c>
       <c r="B233" s="19">
@@ -15064,7 +15008,7 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="36" t="n">
+      <c r="A234" s="35" t="n">
         <v>129.5</v>
       </c>
       <c r="B234" s="19">
@@ -15133,7 +15077,7 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" s="36" t="n">
+      <c r="A235" s="35" t="n">
         <v>130</v>
       </c>
       <c r="B235" s="19">
@@ -15202,7 +15146,7 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="36" t="n">
+      <c r="A236" s="35" t="n">
         <v>130.5</v>
       </c>
       <c r="B236" s="19">
@@ -15271,7 +15215,7 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="36" t="n">
+      <c r="A237" s="35" t="n">
         <v>131</v>
       </c>
       <c r="B237" s="19">
@@ -15340,7 +15284,7 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="36" t="n">
+      <c r="A238" s="35" t="n">
         <v>131.5</v>
       </c>
       <c r="B238" s="19">
@@ -15409,7 +15353,7 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="36" t="n">
+      <c r="A239" s="35" t="n">
         <v>132</v>
       </c>
       <c r="B239" s="19">
@@ -15478,7 +15422,7 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="36" t="n">
+      <c r="A240" s="35" t="n">
         <v>132.5</v>
       </c>
       <c r="B240" s="19">
@@ -15547,7 +15491,7 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="36" t="n">
+      <c r="A241" s="35" t="n">
         <v>133</v>
       </c>
       <c r="B241" s="19">
@@ -15616,7 +15560,7 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="36" t="n">
+      <c r="A242" s="35" t="n">
         <v>133.5</v>
       </c>
       <c r="B242" s="19">
@@ -15685,7 +15629,7 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="36" t="n">
+      <c r="A243" s="35" t="n">
         <v>134</v>
       </c>
       <c r="B243" s="19">
@@ -15754,7 +15698,7 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="36" t="n">
+      <c r="A244" s="35" t="n">
         <v>134.5</v>
       </c>
       <c r="B244" s="19">
@@ -15823,7 +15767,7 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="36" t="n">
+      <c r="A245" s="35" t="n">
         <v>135</v>
       </c>
       <c r="B245" s="19">
@@ -15892,7 +15836,7 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="36" t="n">
+      <c r="A246" s="35" t="n">
         <v>135.5</v>
       </c>
       <c r="B246" s="19">
@@ -15961,7 +15905,7 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="36" t="n">
+      <c r="A247" s="35" t="n">
         <v>136</v>
       </c>
       <c r="B247" s="19">
@@ -16030,7 +15974,7 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="36" t="n">
+      <c r="A248" s="35" t="n">
         <v>136.5</v>
       </c>
       <c r="B248" s="19">
@@ -16099,7 +16043,7 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="36" t="n">
+      <c r="A249" s="35" t="n">
         <v>137</v>
       </c>
       <c r="B249" s="19">
@@ -16168,7 +16112,7 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="36" t="n">
+      <c r="A250" s="35" t="n">
         <v>137.5</v>
       </c>
       <c r="B250" s="19">
@@ -16237,7 +16181,7 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="36" t="n">
+      <c r="A251" s="35" t="n">
         <v>138</v>
       </c>
       <c r="B251" s="19">
@@ -16306,7 +16250,7 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="36" t="n">
+      <c r="A252" s="35" t="n">
         <v>138.5</v>
       </c>
       <c r="B252" s="19">
@@ -16375,7 +16319,7 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="36" t="n">
+      <c r="A253" s="35" t="n">
         <v>139</v>
       </c>
       <c r="B253" s="19">
@@ -16444,7 +16388,7 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="36" t="n">
+      <c r="A254" s="35" t="n">
         <v>139.5</v>
       </c>
       <c r="B254" s="19">
@@ -16513,7 +16457,7 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="36" t="n">
+      <c r="A255" s="35" t="n">
         <v>140</v>
       </c>
       <c r="B255" s="19">

</xml_diff>